<commit_message>
changed labels of building6
</commit_message>
<xml_diff>
--- a/data analysis/data/building6.xlsx
+++ b/data analysis/data/building6.xlsx
@@ -26,15 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Temperature (C)</t>
-  </si>
-  <si>
-    <t>Building 6 kW</t>
   </si>
   <si>
     <t>dayofweek</t>
@@ -365,7 +359,7 @@
   <dimension ref="A1:D365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,13 +374,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5498,7 +5492,7 @@
   <dimension ref="A1:D366"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5508,13 +5502,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10637,7 +10631,7 @@
   <dimension ref="A1:D366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10650,13 +10644,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>